<commit_message>
Updating battery development plot
</commit_message>
<xml_diff>
--- a/Data/Technology_Data.xlsx
+++ b/Data/Technology_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewclarke/Documents/LEADS/CODES/Sustainable_Aviation_Technology_Dashboard/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewclarke/Documents/LEADS/CODES/Technology_Dashboard/Sustainable_Aviation_Technology_Dashboard/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAF3122-F36A-B64D-AE19-71EE1D924F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576FB667-DF6F-2F4D-BAC6-10B3857295C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="72100" yWindow="-4880" windowWidth="30780" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="72100" yWindow="-4880" windowWidth="30780" windowHeight="16020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commercial_Batteries" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
       </extLst>
     </bk>
   </futureMetadata>
-  <futureMetadata name="XLRICHVALUE" count="254">
+  <futureMetadata name="XLRICHVALUE" count="267">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -1843,13 +1843,104 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2048"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2052"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2056"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2059"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2063"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2067"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2070"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2074"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2078"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2081"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2087"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2091"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2093"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
-  <valueMetadata count="254">
+  <valueMetadata count="267">
     <bk>
       <rc t="2" v="0"/>
     </bk>
@@ -2612,12 +2703,51 @@
     <bk>
       <rc t="2" v="253"/>
     </bk>
+    <bk>
+      <rc t="2" v="254"/>
+    </bk>
+    <bk>
+      <rc t="2" v="255"/>
+    </bk>
+    <bk>
+      <rc t="2" v="256"/>
+    </bk>
+    <bk>
+      <rc t="2" v="257"/>
+    </bk>
+    <bk>
+      <rc t="2" v="258"/>
+    </bk>
+    <bk>
+      <rc t="2" v="259"/>
+    </bk>
+    <bk>
+      <rc t="2" v="260"/>
+    </bk>
+    <bk>
+      <rc t="2" v="261"/>
+    </bk>
+    <bk>
+      <rc t="2" v="262"/>
+    </bk>
+    <bk>
+      <rc t="2" v="263"/>
+    </bk>
+    <bk>
+      <rc t="2" v="264"/>
+    </bk>
+    <bk>
+      <rc t="2" v="265"/>
+    </bk>
+    <bk>
+      <rc t="2" v="266"/>
+    </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="417">
   <si>
     <t>Brand</t>
   </si>
@@ -3833,16 +3963,77 @@
   <si>
     <t>Tsukuba</t>
   </si>
+  <si>
+    <t>Ohio State University</t>
+  </si>
+  <si>
+    <t>https://research.cbc.osu.edu/wu.531/research/batteries/</t>
+  </si>
+  <si>
+    <t>Columbus</t>
+  </si>
+  <si>
+    <t>Oklahoma State Universiy</t>
+  </si>
+  <si>
+    <t>https://news.okstate.edu/magazines/engineering-architecture-technology/impact/articles/2021/powering_up.html</t>
+  </si>
+  <si>
+    <t>Stillwater</t>
+  </si>
+  <si>
+    <t>Arizona State University</t>
+  </si>
+  <si>
+    <t>https://news.asu.edu/20230130-asu-startup-receives-funding-advance-firesafe-battery-research</t>
+  </si>
+  <si>
+    <t>https://news.asu.edu/20230714-solid-battery-solution</t>
+  </si>
+  <si>
+    <t>https://arpa-e.energy.gov/technologies/projects/metal-air-electric-vehicle-battery</t>
+  </si>
+  <si>
+    <t>https://economicdevelopment.asu.edu/asu-industries-of-excellence/battery-technology/</t>
+  </si>
+  <si>
+    <t>Tempe</t>
+  </si>
+  <si>
+    <t>Washington University in St. Louis</t>
+  </si>
+  <si>
+    <t>https://source.wustl.edu/2019/07/no-more-trial-and-error-when-choosing-an-electrolyte-for-metal-air-batteries/</t>
+  </si>
+  <si>
+    <t>St. Louis</t>
+  </si>
+  <si>
+    <t>Clemson University</t>
+  </si>
+  <si>
+    <t>https://news.clemson.edu/research-provides-new-insight-into-quantum-effects-in-lithium-sulfur-batteries/</t>
+  </si>
+  <si>
+    <t>Clemson</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3990,28 +4181,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4019,34 +4204,42 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4741,11 +4934,31 @@
     <address r:id="rId259"/>
     <moreImagesAddress r:id="rId260"/>
   </webImageSrd>
+  <webImageSrd>
+    <address r:id="rId261"/>
+    <moreImagesAddress r:id="rId262"/>
+  </webImageSrd>
+  <webImageSrd>
+    <address r:id="rId263"/>
+    <moreImagesAddress r:id="rId264"/>
+  </webImageSrd>
+  <webImageSrd>
+    <address r:id="rId265"/>
+    <moreImagesAddress r:id="rId266"/>
+  </webImageSrd>
+  <webImageSrd>
+    <address r:id="rId267"/>
+    <moreImagesAddress r:id="rId268"/>
+  </webImageSrd>
+  <webImageSrd>
+    <address r:id="rId269"/>
+    <moreImagesAddress r:id="rId270"/>
+  </webImageSrd>
 </webImagesSrd>
 </file>
 
 <file path=xl/richData/rdarray.xml><?xml version="1.0" encoding="utf-8"?>
-<arrayData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="132">
+<arrayData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="135">
   <a r="1">
     <v t="r">6</v>
   </a>
@@ -5504,11 +5717,20 @@
   <a r="1">
     <v t="r">2042</v>
   </a>
+  <a r="1">
+    <v t="r">2053</v>
+  </a>
+  <a r="1">
+    <v t="r">2064</v>
+  </a>
+  <a r="1">
+    <v t="r">2075</v>
+  </a>
 </arrayData>
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2048">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2096">
   <rv s="0">
     <v>536870912</v>
     <v>Suwon</v>
@@ -19698,11 +19920,379 @@
     <v>Tsukuba</v>
     <v>mdp/vdpid/7932726455157391361</v>
   </rv>
+  <rv s="0">
+    <v>536870912</v>
+    <v>Columbus, Ohio</v>
+    <v>5b78da0b-6447-4f71-92b2-f1fafe94ba51</v>
+    <v>en-US</v>
+    <v>Map</v>
+  </rv>
+  <rv s="0">
+    <v>536870912</v>
+    <v>Delaware County</v>
+    <v>342d16f2-de3a-9229-db4d-46d6741911b6</v>
+    <v>en-US</v>
+    <v>Map</v>
+  </rv>
+  <rv s="1">
+    <fb>581.03130599999997</fb>
+    <v>8</v>
+  </rv>
+  <rv s="2">
+    <v>130</v>
+    <v>6</v>
+    <v>407</v>
+    <v>7</v>
+    <v>0</v>
+    <v>Image of Columbus, Ohio</v>
+  </rv>
+  <rv s="1">
+    <fb>39.962222222222202</fb>
+    <v>9</v>
+  </rv>
+  <rv s="0">
+    <v>805306368</v>
+    <v>Andrew Ginther (Mayor)</v>
+    <v>265b4059-0439-3e4a-ef5c-8d2edfb2bf46</v>
+    <v>en-US</v>
+    <v>Generic</v>
+  </rv>
+  <rv s="3">
+    <v>132</v>
+  </rv>
+  <rv s="4">
+    <v>https://www.bing.com/search?q=columbus+ohio&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <fb>-83.000555555555593</fb>
+    <v>9</v>
+  </rv>
+  <rv s="1">
+    <fb>905748</fb>
+    <v>8</v>
+  </rv>
+  <rv s="11">
+    <v>#VALUE!</v>
+    <v>408</v>
+    <v>82</v>
+    <v>Columbus, Ohio</v>
+    <v>4</v>
+    <v>5</v>
+    <v>Map</v>
+    <v>6</v>
+    <v>7</v>
+    <v>en-US</v>
+    <v>5b78da0b-6447-4f71-92b2-f1fafe94ba51</v>
+    <v>536870912</v>
+    <v>1</v>
+    <v>458</v>
+    <v>2049</v>
+    <v>2050</v>
+    <v>367</v>
+    <v>Columbus is the capital and most populous city of the U.S. state of Ohio. With a 2020 census population of 905,748, it is the 14th-most populous city in the U.S., the second-most populous city in the Midwest after Chicago, and the third-most ...</v>
+    <v>2051</v>
+    <v>2052</v>
+    <v>2054</v>
+    <v>2055</v>
+    <v>2056</v>
+    <v>Columbus, Ohio</v>
+    <v>2057</v>
+    <v>Columbus, Ohio</v>
+    <v>mdp/vdpid/5480154750756323330</v>
+  </rv>
+  <rv s="0">
+    <v>536870912</v>
+    <v>Stillwater, Oklahoma</v>
+    <v>9f500d37-adc5-1481-118a-4d2525ba081a</v>
+    <v>en-US</v>
+    <v>Map</v>
+  </rv>
+  <rv s="0">
+    <v>536870912</v>
+    <v>Payne County</v>
+    <v>5cbc7713-d8cb-289f-e378-51787bf0b967</v>
+    <v>en-US</v>
+    <v>Map</v>
+  </rv>
+  <rv s="1">
+    <fb>77.730818999999997</fb>
+    <v>8</v>
+  </rv>
+  <rv s="2">
+    <v>131</v>
+    <v>6</v>
+    <v>409</v>
+    <v>7</v>
+    <v>0</v>
+    <v>Image of Stillwater, Oklahoma</v>
+  </rv>
+  <rv s="1">
+    <fb>36.113444444444397</fb>
+    <v>9</v>
+  </rv>
+  <rv s="0">
+    <v>805306368</v>
+    <v>Will Joyce (Mayor)</v>
+    <v>4e052621-7fcb-4c83-8c85-080762757752</v>
+    <v>en-US</v>
+    <v>Generic</v>
+  </rv>
+  <rv s="3">
+    <v>133</v>
+  </rv>
+  <rv s="4">
+    <v>https://www.bing.com/search?q=stillwater+oklahoma&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <fb>-97.058638888888893</fb>
+    <v>9</v>
+  </rv>
+  <rv s="1">
+    <fb>48394</fb>
+    <v>8</v>
+  </rv>
+  <rv s="16">
+    <v>#VALUE!</v>
+    <v>410</v>
+    <v>118</v>
+    <v>Stillwater, Oklahoma</v>
+    <v>4</v>
+    <v>5</v>
+    <v>Map</v>
+    <v>6</v>
+    <v>7</v>
+    <v>en-US</v>
+    <v>9f500d37-adc5-1481-118a-4d2525ba081a</v>
+    <v>536870912</v>
+    <v>1</v>
+    <v>459</v>
+    <v>2060</v>
+    <v>2061</v>
+    <v>367</v>
+    <v>Stillwater is the tenth-largest city in the U.S. state of Oklahoma. It is the county seat of Payne County, Oklahoma. It is located in north-central Oklahoma at the intersection of U.S. Route 177 and State Highway 51. As of the 2020 census, the ...</v>
+    <v>2062</v>
+    <v>2063</v>
+    <v>2065</v>
+    <v>2066</v>
+    <v>2067</v>
+    <v>Stillwater, Oklahoma</v>
+    <v>2068</v>
+    <v>381</v>
+    <v>Stillwater, Oklahoma</v>
+    <v>mdp/vdpid/5095325061603131393</v>
+  </rv>
+  <rv s="0">
+    <v>536870912</v>
+    <v>Tempe, Arizona</v>
+    <v>47bf306c-e7f2-41f5-a9dd-3e9003176d17</v>
+    <v>en-US</v>
+    <v>Map</v>
+  </rv>
+  <rv s="0">
+    <v>536870912</v>
+    <v>Maricopa County</v>
+    <v>385e4056-0008-58a2-b460-55f838262318</v>
+    <v>en-US</v>
+    <v>Map</v>
+  </rv>
+  <rv s="1">
+    <fb>104.18479600000001</fb>
+    <v>8</v>
+  </rv>
+  <rv s="2">
+    <v>132</v>
+    <v>6</v>
+    <v>411</v>
+    <v>7</v>
+    <v>0</v>
+    <v>Image of Tempe, Arizona</v>
+  </rv>
+  <rv s="1">
+    <fb>33.425555555555597</fb>
+    <v>9</v>
+  </rv>
+  <rv s="0">
+    <v>805306368</v>
+    <v>Corey Woods (Mayor)</v>
+    <v>d64fc925-a214-a079-9320-966014428ea2</v>
+    <v>en-US</v>
+    <v>Generic</v>
+  </rv>
+  <rv s="3">
+    <v>134</v>
+  </rv>
+  <rv s="4">
+    <v>https://www.bing.com/search?q=tempe+arizona&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <fb>-111.94</fb>
+    <v>9</v>
+  </rv>
+  <rv s="1">
+    <fb>180587</fb>
+    <v>8</v>
+  </rv>
+  <rv s="16">
+    <v>#VALUE!</v>
+    <v>412</v>
+    <v>118</v>
+    <v>Tempe, Arizona</v>
+    <v>4</v>
+    <v>5</v>
+    <v>Map</v>
+    <v>6</v>
+    <v>7</v>
+    <v>en-US</v>
+    <v>47bf306c-e7f2-41f5-a9dd-3e9003176d17</v>
+    <v>536870912</v>
+    <v>1</v>
+    <v>426</v>
+    <v>2071</v>
+    <v>2072</v>
+    <v>367</v>
+    <v>Tempe is a city in Maricopa County, Arizona, United States, with the Census Bureau reporting a 2020 population of 180,587. The city is named after the Vale of Tempe in Greece. Tempe is located in the East Valley section of metropolitan Phoenix; ...</v>
+    <v>2073</v>
+    <v>2074</v>
+    <v>2076</v>
+    <v>2077</v>
+    <v>2078</v>
+    <v>Tempe, Arizona</v>
+    <v>2079</v>
+    <v>1420</v>
+    <v>Tempe, Arizona</v>
+    <v>mdp/vdpid/5098091608801280001</v>
+  </rv>
+  <rv s="0">
+    <v>536870912</v>
+    <v>St. Louis</v>
+    <v>e418c908-10a1-4800-815f-406c679d8e13</v>
+    <v>en-US</v>
+    <v>Map</v>
+  </rv>
+  <rv s="1">
+    <fb>171.02625</fb>
+    <v>8</v>
+  </rv>
+  <rv s="2">
+    <v>133</v>
+    <v>6</v>
+    <v>413</v>
+    <v>7</v>
+    <v>0</v>
+    <v>Image of St. Louis</v>
+  </rv>
+  <rv s="4">
+    <v>https://www.bing.com/search?q=st.+louis+missouri&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <fb>301578</fb>
+    <v>8</v>
+  </rv>
+  <rv s="29">
+    <v>#VALUE!</v>
+    <v>414</v>
+    <v>415</v>
+    <v>St. Louis</v>
+    <v>86</v>
+    <v>5</v>
+    <v>Map</v>
+    <v>6</v>
+    <v>7</v>
+    <v>en-US</v>
+    <v>e418c908-10a1-4800-815f-406c679d8e13</v>
+    <v>536870912</v>
+    <v>1</v>
+    <v>448</v>
+    <v>2082</v>
+    <v>367</v>
+    <v>St. Louis is an independent city in the U.S. state of Missouri. It is located near the confluence of the Mississippi and the Missouri rivers. In 2020, the city proper had a population of 301,578, while its bi-state metropolitan area, which ...</v>
+    <v>2083</v>
+    <v>2084</v>
+    <v>St. Louis</v>
+    <v>2085</v>
+    <v>381</v>
+    <v>St. Louis</v>
+    <v>mdp/vdpid/5096642009372819458</v>
+  </rv>
+  <rv s="0">
+    <v>536870912</v>
+    <v>Clemson, South Carolina</v>
+    <v>ec1c5457-2e06-5604-5b11-17822106b236</v>
+    <v>en-US</v>
+    <v>Map</v>
+  </rv>
+  <rv s="0">
+    <v>536870912</v>
+    <v>Pickens County</v>
+    <v>d71b1ca3-732a-dca6-70e3-11a1880b2026</v>
+    <v>en-US</v>
+    <v>Map</v>
+  </rv>
+  <rv s="1">
+    <fb>20.384834000000001</fb>
+    <v>8</v>
+  </rv>
+  <rv s="2">
+    <v>134</v>
+    <v>6</v>
+    <v>416</v>
+    <v>7</v>
+    <v>0</v>
+    <v>Image of Clemson, South Carolina</v>
+  </rv>
+  <rv s="1">
+    <fb>34.685000000000002</fb>
+    <v>9</v>
+  </rv>
+  <rv s="4">
+    <v>https://www.bing.com/search?q=clemson+sc&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <fb>-82.814722222222002</fb>
+    <v>9</v>
+  </rv>
+  <rv s="1">
+    <fb>17681</fb>
+    <v>8</v>
+  </rv>
+  <rv s="18">
+    <v>#VALUE!</v>
+    <v>417</v>
+    <v>132</v>
+    <v>Clemson, South Carolina</v>
+    <v>4</v>
+    <v>5</v>
+    <v>Map</v>
+    <v>6</v>
+    <v>7</v>
+    <v>en-US</v>
+    <v>ec1c5457-2e06-5604-5b11-17822106b236</v>
+    <v>536870912</v>
+    <v>1</v>
+    <v>464</v>
+    <v>2088</v>
+    <v>2089</v>
+    <v>367</v>
+    <v>Clemson is a city in Pickens and Anderson counties in the U.S. state of South Carolina. Clemson is home to Clemson University; in 2015, the Princeton Review cited the town of Clemson as ranking #1 in the United States for "town-and-gown" ...</v>
+    <v>2090</v>
+    <v>2091</v>
+    <v>2092</v>
+    <v>2093</v>
+    <v>Clemson, South Carolina</v>
+    <v>2094</v>
+    <v>Clemson, South Carolina</v>
+    <v>mdp/vdpid/5484700030239506433</v>
+  </rv>
 </rvData>
 </file>
 
 <file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="29">
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="30">
   <s t="_linkedentity2">
     <k n="%EntityServiceId" t="i"/>
     <k n="_DisplayString" t="s"/>
@@ -20620,12 +21210,38 @@
     <k n="Urban population" t="r"/>
     <k n="VDPID/VSID" t="s"/>
   </s>
+  <s t="_linkedentity2core">
+    <k n="_CRID" t="e"/>
+    <k n="_Attribution" t="spb"/>
+    <k n="_Display" t="spb"/>
+    <k n="_DisplayString" t="s"/>
+    <k n="_Flags" t="spb"/>
+    <k n="_Format" t="spb"/>
+    <k n="_Icon" t="s"/>
+    <k n="_Provider" t="spb"/>
+    <k n="_SubLabel" t="spb"/>
+    <k n="%EntityCulture" t="s"/>
+    <k n="%EntityId" t="s"/>
+    <k n="%EntityServiceId" t="i"/>
+    <k n="%IsRefreshable" t="b"/>
+    <k n="Admin Division 1 (State/province/other)" t="r"/>
+    <k n="Area" t="r"/>
+    <k n="Country/region" t="r"/>
+    <k n="Description" t="s"/>
+    <k n="Image" t="r"/>
+    <k n="LearnMoreOnLink" t="r"/>
+    <k n="Name" t="s"/>
+    <k n="Population" t="r"/>
+    <k n="Time zone(s)" t="r"/>
+    <k n="UniqueName" t="s"/>
+    <k n="VDPID/VSID" t="s"/>
+  </s>
 </rvStructures>
 </file>
 
 <file path=xl/richData/rdsupportingpropertybag.xml><?xml version="1.0" encoding="utf-8"?>
 <supportingPropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
-  <spbArrays count="24">
+  <spbArrays count="25">
     <a count="25">
       <v t="s">%EntityServiceId</v>
       <v t="s">%IsRefreshable</v>
@@ -21494,8 +22110,33 @@
       <v t="s">Image</v>
       <v t="s">Description</v>
     </a>
+    <a count="23">
+      <v t="s">%EntityServiceId</v>
+      <v t="s">%IsRefreshable</v>
+      <v t="s">%EntityCulture</v>
+      <v t="s">%EntityId</v>
+      <v t="s">_Icon</v>
+      <v t="s">_Provider</v>
+      <v t="s">_Attribution</v>
+      <v t="s">_Display</v>
+      <v t="s">Name</v>
+      <v t="s">_Format</v>
+      <v t="s">Admin Division 1 (State/province/other)</v>
+      <v t="s">Country/region</v>
+      <v t="s">_SubLabel</v>
+      <v t="s">Population</v>
+      <v t="s">Area</v>
+      <v t="s">_Flags</v>
+      <v t="s">VDPID/VSID</v>
+      <v t="s">UniqueName</v>
+      <v t="s">_DisplayString</v>
+      <v t="s">LearnMoreOnLink</v>
+      <v t="s">Time zone(s)</v>
+      <v t="s">Image</v>
+      <v t="s">Description</v>
+    </a>
   </spbArrays>
-  <spbData count="407">
+  <spbData count="418">
     <spb s="0">
       <v xml:space="preserve">Wikipedia	</v>
       <v xml:space="preserve">CC BY-SA 3.0	</v>
@@ -25503,6 +26144,98 @@
       <v>405</v>
       <v>405</v>
     </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	</v>
+      <v xml:space="preserve">CC BY-SA 3.0	</v>
+      <v xml:space="preserve">https://en.wikipedia.org/wiki/Columbus,_Ohio	</v>
+      <v xml:space="preserve">https://creativecommons.org/licenses/by-sa/3.0	</v>
+    </spb>
+    <spb s="18">
+      <v>407</v>
+      <v>407</v>
+      <v>407</v>
+      <v>407</v>
+      <v>407</v>
+      <v>407</v>
+      <v>407</v>
+      <v>407</v>
+      <v>407</v>
+      <v>407</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	</v>
+      <v xml:space="preserve">CC BY-SA 3.0	</v>
+      <v xml:space="preserve">https://en.wikipedia.org/wiki/Stillwater,_Oklahoma	</v>
+      <v xml:space="preserve">https://creativecommons.org/licenses/by-sa/3.0	</v>
+    </spb>
+    <spb s="18">
+      <v>409</v>
+      <v>409</v>
+      <v>409</v>
+      <v>409</v>
+      <v>409</v>
+      <v>409</v>
+      <v>409</v>
+      <v>409</v>
+      <v>409</v>
+      <v>409</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	</v>
+      <v xml:space="preserve">CC BY-SA 3.0	</v>
+      <v xml:space="preserve">https://en.wikipedia.org/wiki/Tempe,_Arizona	</v>
+      <v xml:space="preserve">https://creativecommons.org/licenses/by-sa/3.0	</v>
+    </spb>
+    <spb s="18">
+      <v>411</v>
+      <v>411</v>
+      <v>411</v>
+      <v>411</v>
+      <v>411</v>
+      <v>411</v>
+      <v>411</v>
+      <v>411</v>
+      <v>411</v>
+      <v>411</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	</v>
+      <v xml:space="preserve">CC BY-SA 3.0	</v>
+      <v xml:space="preserve">https://en.wikipedia.org/wiki/St._Louis	</v>
+      <v xml:space="preserve">https://creativecommons.org/licenses/by-sa/3.0	</v>
+    </spb>
+    <spb s="26">
+      <v>413</v>
+      <v>413</v>
+      <v>413</v>
+      <v>413</v>
+      <v>413</v>
+      <v>413</v>
+      <v>413</v>
+    </spb>
+    <spb s="2">
+      <v>24</v>
+      <v>Name</v>
+      <v>LearnMoreOnLink</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	</v>
+      <v xml:space="preserve">CC BY-SA 3.0	</v>
+      <v xml:space="preserve">https://en.wikipedia.org/wiki/Clemson,_South_Carolina	</v>
+      <v xml:space="preserve">https://creativecommons.org/licenses/by-sa/3.0	</v>
+    </spb>
+    <spb s="18">
+      <v>416</v>
+      <v>416</v>
+      <v>416</v>
+      <v>416</v>
+      <v>416</v>
+      <v>416</v>
+      <v>416</v>
+      <v>416</v>
+      <v>416</v>
+      <v>416</v>
+    </spb>
   </spbData>
 </supportingPropertyBags>
 </file>
@@ -26382,8 +27115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE911"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -58569,9 +59302,9 @@
   </sheetPr>
   <dimension ref="A1:AF989"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
+      <selection pane="bottomLeft" activeCell="E112" sqref="E112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -62871,21 +63604,216 @@
       </c>
     </row>
     <row r="104" spans="1:15" ht="16">
-      <c r="A104" s="15"/>
-      <c r="K104" s="23"/>
-      <c r="M104" s="22"/>
+      <c r="A104" s="24" t="s">
+        <v>399</v>
+      </c>
+      <c r="B104" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="C104" s="24">
+        <v>0</v>
+      </c>
+      <c r="E104" s="24">
+        <v>0</v>
+      </c>
+      <c r="G104" s="24">
+        <v>1</v>
+      </c>
+      <c r="H104" s="25" t="s">
+        <v>400</v>
+      </c>
+      <c r="I104" s="24">
+        <v>0</v>
+      </c>
+      <c r="K104" s="24" t="s">
+        <v>401</v>
+      </c>
+      <c r="L104" s="24" t="e" vm="255">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M104" s="22" t="e" cm="1" vm="15">
+        <f t="array" ref="M104">_FV( L104,"Country/region",TRUE)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N104" cm="1" vm="256">
+        <f t="array" ref="N104">_FV( L104,"Latitude")</f>
+        <v>39.962222222222202</v>
+      </c>
+      <c r="O104" cm="1" vm="257">
+        <f t="array" ref="O104">_FV( L104,"Longitude")</f>
+        <v>-83.000555555555593</v>
+      </c>
     </row>
     <row r="105" spans="1:15" ht="15" customHeight="1">
-      <c r="K105" s="23"/>
+      <c r="A105" s="24" t="s">
+        <v>402</v>
+      </c>
+      <c r="B105" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="C105" s="24">
+        <v>0</v>
+      </c>
+      <c r="E105" s="24">
+        <v>0</v>
+      </c>
+      <c r="G105" s="24">
+        <v>1</v>
+      </c>
+      <c r="H105" s="25" t="s">
+        <v>403</v>
+      </c>
+      <c r="I105" s="24">
+        <v>0</v>
+      </c>
+      <c r="K105" s="24" t="s">
+        <v>404</v>
+      </c>
+      <c r="L105" s="24" t="e" vm="258">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M105" s="22" t="e" cm="1" vm="15">
+        <f t="array" ref="M105">_FV( L105,"Country/region",TRUE)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N105" cm="1" vm="259">
+        <f t="array" ref="N105">_FV( L105,"Latitude")</f>
+        <v>36.113444444444397</v>
+      </c>
+      <c r="O105" cm="1" vm="260">
+        <f t="array" ref="O105">_FV( L105,"Longitude")</f>
+        <v>-97.058638888888893</v>
+      </c>
     </row>
     <row r="106" spans="1:15" ht="15" customHeight="1">
-      <c r="K106" s="23"/>
+      <c r="A106" s="24" t="s">
+        <v>405</v>
+      </c>
+      <c r="B106" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="C106" s="24">
+        <v>1</v>
+      </c>
+      <c r="D106" s="25" t="s">
+        <v>406</v>
+      </c>
+      <c r="E106" s="24">
+        <v>1</v>
+      </c>
+      <c r="F106" s="25" t="s">
+        <v>407</v>
+      </c>
+      <c r="G106" s="24">
+        <v>1</v>
+      </c>
+      <c r="H106" s="25" t="s">
+        <v>408</v>
+      </c>
+      <c r="I106" s="24">
+        <v>1</v>
+      </c>
+      <c r="J106" s="25" t="s">
+        <v>409</v>
+      </c>
+      <c r="K106" s="24" t="s">
+        <v>410</v>
+      </c>
+      <c r="L106" s="24" t="e" vm="261">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M106" s="22" t="e" cm="1" vm="15">
+        <f t="array" ref="M106">_FV( L106,"Country/region",TRUE)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N106" cm="1" vm="262">
+        <f t="array" ref="N106">_FV( L106,"Latitude")</f>
+        <v>33.425555555555597</v>
+      </c>
+      <c r="O106" cm="1" vm="263">
+        <f t="array" ref="O106">_FV( L106,"Longitude")</f>
+        <v>-111.94</v>
+      </c>
     </row>
     <row r="107" spans="1:15" ht="15" customHeight="1">
-      <c r="K107" s="23"/>
+      <c r="A107" s="24" t="s">
+        <v>411</v>
+      </c>
+      <c r="B107" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="C107" s="24">
+        <v>0</v>
+      </c>
+      <c r="E107" s="24">
+        <v>0</v>
+      </c>
+      <c r="G107" s="24">
+        <v>1</v>
+      </c>
+      <c r="H107" s="25" t="s">
+        <v>412</v>
+      </c>
+      <c r="I107" s="24">
+        <v>0</v>
+      </c>
+      <c r="K107" s="24" t="s">
+        <v>413</v>
+      </c>
+      <c r="L107" s="24" t="e" vm="264">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M107" s="22" t="e" cm="1" vm="15">
+        <f t="array" ref="M107">_FV( L107,"Country/region",TRUE)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N107">
+        <v>38.648336998842801</v>
+      </c>
+      <c r="O107">
+        <v>-90.310796203077999</v>
+      </c>
     </row>
     <row r="108" spans="1:15" ht="15" customHeight="1">
-      <c r="K108" s="23"/>
+      <c r="A108" s="24" t="s">
+        <v>414</v>
+      </c>
+      <c r="B108" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="C108" s="24">
+        <v>0</v>
+      </c>
+      <c r="E108" s="24">
+        <v>1</v>
+      </c>
+      <c r="F108" s="25" t="s">
+        <v>415</v>
+      </c>
+      <c r="G108" s="24">
+        <v>0</v>
+      </c>
+      <c r="I108" s="24">
+        <v>0</v>
+      </c>
+      <c r="K108" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="L108" s="24" t="e" vm="265">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M108" s="22" t="e" cm="1" vm="15">
+        <f t="array" ref="M108">_FV( L108,"Country/region",TRUE)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N108" cm="1" vm="266">
+        <f t="array" ref="N108">_FV( L108,"Latitude")</f>
+        <v>34.685000000000002</v>
+      </c>
+      <c r="O108" cm="1" vm="267">
+        <f t="array" ref="O108">_FV( L108,"Longitude")</f>
+        <v>-82.814722222222002</v>
+      </c>
     </row>
     <row r="109" spans="1:15" ht="15" customHeight="1">
       <c r="K109" s="23"/>
@@ -65639,6 +66567,14 @@
     <hyperlink ref="D19" r:id="rId105" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
     <hyperlink ref="D18" r:id="rId106" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
     <hyperlink ref="D17" r:id="rId107" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="H104" r:id="rId108" xr:uid="{381C9651-AA38-3548-A551-2F4EA126DC40}"/>
+    <hyperlink ref="H105" r:id="rId109" xr:uid="{ABC3E85C-738F-624F-BECD-F808E1B088D4}"/>
+    <hyperlink ref="D106" r:id="rId110" xr:uid="{E9A92998-E005-3848-9564-2756C6622365}"/>
+    <hyperlink ref="F106" r:id="rId111" xr:uid="{C051F18C-97F7-5943-A317-FB231D5607F0}"/>
+    <hyperlink ref="H106" r:id="rId112" xr:uid="{CC93508F-B29D-F945-B0BC-C0F143D5C177}"/>
+    <hyperlink ref="J106" r:id="rId113" xr:uid="{EB4FB63A-0839-CE43-B142-E9B6504301E3}"/>
+    <hyperlink ref="H107" r:id="rId114" xr:uid="{38EBDE14-90F3-644D-B009-5AA10FAA274B}"/>
+    <hyperlink ref="F108" r:id="rId115" xr:uid="{288650BB-1512-E04A-8B68-2DDA76F20672}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>